<commit_message>
Added support for intelliJ IDE
</commit_message>
<xml_diff>
--- a/ExcelOp/src/myPackage/myExcel.xlsx
+++ b/ExcelOp/src/myPackage/myExcel.xlsx
@@ -64,17 +64,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>

</xml_diff>